<commit_message>
Updated Excel input file.
Revenue projections now reflect Clinton CTC update.
</commit_message>
<xml_diff>
--- a/Parameters/RevenuesPctGDP_ToJorge.xlsx
+++ b/Parameters/RevenuesPctGDP_ToJorge.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\DynamicModel\Dev_jbarro\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnon\Documents\Projects\TaxPolicySim\Inputs\TPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13335"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15630" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -408,7 +408,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -450,7 +450,7 @@
         <v>18.406860000000002</v>
       </c>
       <c r="C3" s="4">
-        <v>18.406860000000002</v>
+        <v>18.406863006094078</v>
       </c>
       <c r="D3" s="4">
         <v>18.406860000000002</v>
@@ -467,7 +467,7 @@
         <v>18.101610000000001</v>
       </c>
       <c r="C4" s="4">
-        <v>18.160019999999999</v>
+        <v>18.160015296595475</v>
       </c>
       <c r="D4" s="4">
         <v>18.061530000000001</v>
@@ -484,7 +484,7 @@
         <v>18.200189999999999</v>
       </c>
       <c r="C5" s="4">
-        <v>18.63298</v>
+        <v>18.517215569811132</v>
       </c>
       <c r="D5" s="4">
         <v>15.164910000000001</v>
@@ -501,7 +501,7 @@
         <v>18.093830000000001</v>
       </c>
       <c r="C6" s="4">
-        <v>18.611789999999999</v>
+        <v>18.501408786788229</v>
       </c>
       <c r="D6" s="4">
         <v>15.198689999999999</v>
@@ -518,7 +518,7 @@
         <v>18.019189999999998</v>
       </c>
       <c r="C7" s="4">
-        <v>18.618490000000001</v>
+        <v>18.51288048582191</v>
       </c>
       <c r="D7" s="4">
         <v>15.20196</v>
@@ -535,7 +535,7 @@
         <v>18.124610000000001</v>
       </c>
       <c r="C8" s="4">
-        <v>18.726400000000002</v>
+        <v>18.626240949857507</v>
       </c>
       <c r="D8" s="4">
         <v>15.172739999999999</v>
@@ -552,7 +552,7 @@
         <v>18.038900000000002</v>
       </c>
       <c r="C9" s="4">
-        <v>18.66985</v>
+        <v>18.575050498562437</v>
       </c>
       <c r="D9" s="4">
         <v>15.381919999999999</v>
@@ -569,7 +569,7 @@
         <v>18.052019999999999</v>
       </c>
       <c r="C10" s="4">
-        <v>18.71518</v>
+        <v>18.625631473037672</v>
       </c>
       <c r="D10" s="4">
         <v>15.376860000000001</v>
@@ -586,7 +586,7 @@
         <v>18.054819999999999</v>
       </c>
       <c r="C11" s="4">
-        <v>18.730550000000001</v>
+        <v>18.645986046475375</v>
       </c>
       <c r="D11" s="4">
         <v>15.497769999999999</v>
@@ -603,7 +603,7 @@
         <v>18.1004</v>
       </c>
       <c r="C12" s="4">
-        <v>18.786860000000001</v>
+        <v>18.707127769652164</v>
       </c>
       <c r="D12" s="4">
         <v>15.481619999999999</v>
@@ -620,7 +620,7 @@
         <v>18.182200000000002</v>
       </c>
       <c r="C13" s="4">
-        <v>18.8767</v>
+        <v>18.801497904249576</v>
       </c>
       <c r="D13" s="4">
         <v>15.604480000000001</v>
@@ -637,7 +637,7 @@
         <v>18.23602</v>
       </c>
       <c r="C14" s="4">
-        <v>18.940180000000002</v>
+        <v>18.868966720585707</v>
       </c>
       <c r="D14" s="4">
         <v>15.601129999999999</v>
@@ -654,7 +654,7 @@
         <v>18.204560000000001</v>
       </c>
       <c r="C15" s="4">
-        <v>18.917570000000001</v>
+        <v>18.851037852570972</v>
       </c>
       <c r="D15" s="4">
         <v>15.564579999999999</v>
@@ -671,7 +671,7 @@
         <v>18.314859999999999</v>
       </c>
       <c r="C16" s="4">
-        <v>19.033760000000001</v>
+        <v>18.970076554976252</v>
       </c>
       <c r="D16" s="4">
         <v>15.68676</v>
@@ -688,7 +688,7 @@
         <v>18.389869999999998</v>
       </c>
       <c r="C17" s="4">
-        <v>19.115069999999999</v>
+        <v>19.054455820249423</v>
       </c>
       <c r="D17" s="4">
         <v>15.790789999999999</v>
@@ -705,7 +705,7 @@
         <v>18.380510000000001</v>
       </c>
       <c r="C18" s="4">
-        <v>19.110279999999999</v>
+        <v>19.051898093245796</v>
       </c>
       <c r="D18" s="4">
         <v>15.797359999999999</v>
@@ -722,7 +722,7 @@
         <v>18.520340000000001</v>
       </c>
       <c r="C19" s="4">
-        <v>19.260670000000001</v>
+        <v>19.20556643427738</v>
       </c>
       <c r="D19" s="4">
         <v>15.953749999999999</v>
@@ -739,7 +739,7 @@
         <v>18.470469999999999</v>
       </c>
       <c r="C20" s="4">
-        <v>19.221340000000001</v>
+        <v>19.169319891986099</v>
       </c>
       <c r="D20" s="4">
         <v>15.9129</v>
@@ -756,7 +756,7 @@
         <v>18.613040000000002</v>
       </c>
       <c r="C21" s="4">
-        <v>19.374400000000001</v>
+        <v>19.325287829431627</v>
       </c>
       <c r="D21" s="4">
         <v>16.06437</v>
@@ -773,7 +773,7 @@
         <v>18.68402</v>
       </c>
       <c r="C22" s="4">
-        <v>19.4558</v>
+        <v>19.40941223991031</v>
       </c>
       <c r="D22" s="4">
         <v>16.140840000000001</v>
@@ -790,7 +790,7 @@
         <v>18.666090000000001</v>
       </c>
       <c r="C23" s="4">
-        <v>19.448170000000001</v>
+        <v>19.404358430568255</v>
       </c>
       <c r="D23" s="4">
         <v>16.127600000000001</v>
@@ -807,7 +807,7 @@
         <v>18.788409999999999</v>
       </c>
       <c r="C24" s="4">
-        <v>19.580639999999999</v>
+        <v>19.539252365850686</v>
       </c>
       <c r="D24" s="4">
         <v>16.25309</v>
@@ -824,7 +824,7 @@
         <v>18.8658</v>
       </c>
       <c r="C25" s="4">
-        <v>19.66799</v>
+        <v>19.628883722401753</v>
       </c>
       <c r="D25" s="4">
         <v>16.33211</v>
@@ -841,7 +841,7 @@
         <v>18.856359999999999</v>
       </c>
       <c r="C26" s="4">
-        <v>19.66827</v>
+        <v>19.631312428188032</v>
       </c>
       <c r="D26" s="4">
         <v>16.32274</v>
@@ -858,7 +858,7 @@
         <v>18.975190000000001</v>
       </c>
       <c r="C27" s="4">
-        <v>19.79654</v>
+        <v>19.761607379743378</v>
       </c>
       <c r="D27" s="4">
         <v>16.44106</v>
@@ -875,7 +875,7 @@
         <v>18.942440000000001</v>
       </c>
       <c r="C28" s="4">
-        <v>19.772880000000001</v>
+        <v>19.739861281698794</v>
       </c>
       <c r="D28" s="4">
         <v>16.407779999999999</v>

</xml_diff>